<commit_message>
analyse and design doc
</commit_message>
<xml_diff>
--- a/xml_translatin.xlsx
+++ b/xml_translatin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="269">
   <si>
     <t>name</t>
   </si>
@@ -47,27 +47,6 @@
     <t>digits_number_of_phonenumber_must_be_11</t>
   </si>
   <si>
-    <t>phonenumber should not start with 0 digit!</t>
-  </si>
-  <si>
-    <t>phonenumber_should_not_start_with_0_digit</t>
-  </si>
-  <si>
-    <t>شماره تلفن نباید با صفر شروع شود.</t>
-  </si>
-  <si>
-    <t>digits number of phonenumber must be 8!</t>
-  </si>
-  <si>
-    <t>digits_number_of_phonenumber_must be_8</t>
-  </si>
-  <si>
-    <t>digits number of phonenumber must be between 3 and 8!</t>
-  </si>
-  <si>
-    <t>digits_number_of_phonenumber_must_be_between_3_and_8</t>
-  </si>
-  <si>
     <t>ارقام شماره تلفن وارد شده باید  بین 3 تا 8 باشد.</t>
   </si>
   <si>
@@ -360,13 +339,505 @@
   </si>
   <si>
     <t>user_deactivation_was_unsuccessful</t>
+  </si>
+  <si>
+    <t>Access/user file</t>
+  </si>
+  <si>
+    <t>Err_get_user_by_id:_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err get user by id: id is not valid!</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش اطلاعات کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit User: user id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_User:_user_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>در ویرایش اطلاعات کاربر باید حداقل یک پارامتر تعیین شود!</t>
+  </si>
+  <si>
+    <t>msg edit user: you should specify at least one parameter!</t>
+  </si>
+  <si>
+    <t>edit user profile information was successful.</t>
+  </si>
+  <si>
+    <t>ویرایش اطلاعات پروفایل کاربر با موفقیت انجام شد.</t>
+  </si>
+  <si>
+    <t>edit_user_profile_information_was_successful</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش گذرواژه: شناسه کاربر معتبر نیست!</t>
+  </si>
+  <si>
+    <t>msg edit password: user id is not valid!</t>
+  </si>
+  <si>
+    <t>msg_edit_password:_user_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش گذرواژه: گذرواژه وارد نشده است!</t>
+  </si>
+  <si>
+    <t>msg password edit: password not set!</t>
+  </si>
+  <si>
+    <t>msg_password_edit:_password_not_set</t>
+  </si>
+  <si>
+    <t>msg_edit_user:_you_should_specify_at_least_one_parameter</t>
+  </si>
+  <si>
+    <t>خطا در حذف کاربر: شناسه کاربر معتبر نیست!</t>
+  </si>
+  <si>
+    <t>Err delete user by id: id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_delete_user_by_id_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در فعال‌سازی کاربر: شناسه کاربر معتبر نیست!</t>
+  </si>
+  <si>
+    <t>Err_activate_user:_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در غیرفعال‌سازی کاربر: شناسه کاربر معتبر نیست!</t>
+  </si>
+  <si>
+    <t>Err_deactivate_user:_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err deactivate user: id is not valid!</t>
+  </si>
+  <si>
+    <t>Err activate user: id is not valid!</t>
+  </si>
+  <si>
+    <t>Err check user lost password: id is not valid</t>
+  </si>
+  <si>
+    <t>خطا در بررسی از دست رفتن گذرواژه کاربر: شناسه کاربر معتبر نیست!</t>
+  </si>
+  <si>
+    <t>Err_check_user_lost_password:_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: نام کاربری مورد نظر ثبت نشده است!</t>
+  </si>
+  <si>
+    <t>Err login: This Username have not registered!</t>
+  </si>
+  <si>
+    <t>Err_login:_This_Username_have_not_registered</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: گذرواژه و پسورد شما اشتباه است!</t>
+  </si>
+  <si>
+    <t>Err login: Your username and password not correct!</t>
+  </si>
+  <si>
+    <t>Err_login:_Your_username_and_password_not_correct</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: برای این کاربر دسترسی وجود ندارد!</t>
+  </si>
+  <si>
+    <t>msg login: no action list found for this user!</t>
+  </si>
+  <si>
+    <t>msg_login:_no_action_list_found_for_this_user</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: در این سیستم اجازه ورود ندارید!</t>
+  </si>
+  <si>
+    <t>Err login: You have not access to login in system!</t>
+  </si>
+  <si>
+    <t>Err_login:_You_have_not_access_to_login_in_system</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: حساب کاربری شما مسدود است!</t>
+  </si>
+  <si>
+    <t>msg login : your account has been blocked!</t>
+  </si>
+  <si>
+    <t>msg_login:_your_account_has_been_blocked</t>
+  </si>
+  <si>
+    <t>خطا در ورود کاربر: حساب کاربری شما پیش‌تر پاک حذف شده است!</t>
+  </si>
+  <si>
+    <t>msg login: your account has been deleted before!</t>
+  </si>
+  <si>
+    <t>msg_login:_your_account_has_been_deleted_before</t>
+  </si>
+  <si>
+    <t>خطا در خروج کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>msg logout: User id is not valid!</t>
+  </si>
+  <si>
+    <t>msg_logout:_User_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی نقش کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err get user role: Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err get user profile: Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_user_profile:_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err_get_user_role:_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی گروه کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err get user group: Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_user_group:_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ثبت پروفایل کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>"Err set user profile: Id is not valid!</t>
+  </si>
+  <si>
+    <t>"Err_set_user_profile:_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err get user role: user id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_user_role:_user_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی نقش کاربر: شناسه نقش معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err get user role: role id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_user_role:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>شما باید حداقل یک پارامتر را تعیین نمایید!</t>
+  </si>
+  <si>
+    <t>You should specify at least one parameter!</t>
+  </si>
+  <si>
+    <t>You_should_specify_at_least_one_parameter</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش پروفایل کاربر: شناسه کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_user_profile: User Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_user_profile:_User_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش پروفایل کاربر: هیچ کاربر معتبری برای این شناسه وجود ندارد!</t>
+  </si>
+  <si>
+    <t>Err edit user profile: no Valid user for this id!</t>
+  </si>
+  <si>
+    <t>Err_edit_user_profile:_no_Valid_user_for_this_id</t>
+  </si>
+  <si>
+    <t>Err get role: role id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_role:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش نقش کاربر: شناسه نقش معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_role: Role Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_role:_Role_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی عمل: شناسه‌ی عمل معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err_get_action:_action_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err get action: action id is not valid!</t>
+  </si>
+  <si>
+    <t>Edit Action: You should specify at least One parameter!</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش عمل: شما باید حداقل یک پارامتر را تعیین نمایید!</t>
+  </si>
+  <si>
+    <t>Edit Action: You_should_specify_at_least_One_parameter</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش عمل: شناسه عمل معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_action: action Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_action:_action_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در حذف عمل: شناسه عمل معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err delete action: action id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_delete_action:_action_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ثبت عمل دسترسی: شناسه عمل معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err set role action: action id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_set_role_action:_action_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>بازیابی عمل دسترسی: شناسه دسترسی معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>msg get role action: role id is not valid!</t>
+  </si>
+  <si>
+    <t>msg_get_role_action:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در حذف دسترسی: شناسه‌ی دسترسی معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err_delete_role:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err delete role:role id is not valid!</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی گروه: شناسه‌ی گروه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err get group: group id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_group:_group_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش گروه: شما باید حداقل یک پارامتر را تعیین نمایید!</t>
+  </si>
+  <si>
+    <t>Edit Group: You should specify at least one of the parameters!</t>
+  </si>
+  <si>
+    <t>Edit_Group:_You_should_specify_at_least_one_of_the_parameters</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش گروه: شناسه‌ی گروه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_group: group Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_group:_group_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در حذف گروه: شناسه‌ی گروه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err delete group: group id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_delete_group:_group_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش شهر: شما باید حداقل یک پارامتر را تعیین نمایید!</t>
+  </si>
+  <si>
+    <t>Err edit_city: You should specify at least one parameter!</t>
+  </si>
+  <si>
+    <t>Err_edit_city:_You_should_specify_at_least_one_parameter</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش شهر: شناسه‌ی شهر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_City: City Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_City:_City_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش شهر: شناسه‌ی استان معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_City: State Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_City:_Stat_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err delete_City: city Id is not valid!</t>
+  </si>
+  <si>
+    <t>خطا در حذف شهر: شناسه‌ی شهر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err_delete_City:_city_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در بازیابی منطقه: شناسه‌ی منطقه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err get region by id: region id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_get_region_by_id:_region_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش منطقه: شما باید حداقل یک پارامتر را تعیین نمایید!</t>
+  </si>
+  <si>
+    <t>Err edit_region: You should specify at least one parameter!</t>
+  </si>
+  <si>
+    <t>Err_edit_region:_You_should_specify_at_least_one_parameter</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش منطقه: شناسه‌ی منطقه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err edit_region: region Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_edit_region:_region_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err edit_Region: City Id is not valid</t>
+  </si>
+  <si>
+    <t>خطا در ویرایش منطقه: شناسه‌ی شهر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>خطا در حذف منطقه: شناسه‌ی منطقه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err delete_Region: region Id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_delete_Region:_region_Id_is_not_valid</t>
+  </si>
+  <si>
+    <t>خطا در ثبت گروه دسترسی: شناسه‌ی دسترسی معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err set role group: role id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_set_role_group:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err set role group: group id is not valid</t>
+  </si>
+  <si>
+    <t>خطا در ثبت گروه دسترسی: شناسه‌ی گروه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err delete role group: role id is not valid</t>
+  </si>
+  <si>
+    <t>خطا در حذف گروه دسترسی: شناسه‌ی دسترسی معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>خطا در حذف گروه دسترسی: شناسه‌ی گروه معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err delete role group: group id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_delete_role_group:_group_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err_delete_role_group:_role_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err_set_role_group:_group_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>Err set user group: user id is not valid</t>
+  </si>
+  <si>
+    <t>خطا در ثبت گروه کاربر: شناسه‌ی کاربر معتبر نمی‌باشد!</t>
+  </si>
+  <si>
+    <t>Err set user group: user id is not valid!</t>
+  </si>
+  <si>
+    <t>Err_set_user _group:_user_id_is_not_valid</t>
+  </si>
+  <si>
+    <t>phonenumber should not start with 0 or 1 digits!</t>
+  </si>
+  <si>
+    <t>phonenumber_should_not_start_with_0_or_1_digits</t>
+  </si>
+  <si>
+    <t>شماره تلفن نباید با صفر یا یک شروع شود!</t>
+  </si>
+  <si>
+    <t>digit numbers of phonenumber must be between 3 and 8!</t>
+  </si>
+  <si>
+    <t>digit_numbers_of_phonenumber_must_be_between_3_and_8</t>
+  </si>
+  <si>
+    <t>digit_numbers_of_phonenumber_must be_8</t>
+  </si>
+  <si>
+    <t>digit numbers of phonenumber must be 8!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +877,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -427,7 +904,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -437,6 +914,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,11 +1197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,240 +1223,240 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
+      <c r="A3" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>263</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>262</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>267</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>268</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>266</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>265</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -986,7 +1466,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1"/>
     </row>
@@ -995,183 +1475,807 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="C43" s="2"/>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="4"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
last update in satrday
</commit_message>
<xml_diff>
--- a/xml_translatin.xlsx
+++ b/xml_translatin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="275">
   <si>
     <t>name</t>
   </si>
@@ -840,6 +840,15 @@
   </si>
   <si>
     <t>You_are_logged_out_successfully.</t>
+  </si>
+  <si>
+    <t>your description is so long!</t>
+  </si>
+  <si>
+    <t>توضیحات شما بسیار طولانی است!</t>
+  </si>
+  <si>
+    <t>your_description_is_so_long</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,854 +1457,865 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>274</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>51</v>
+        <v>272</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="B27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>271</v>
+        <v>98</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>270</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>269</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>116</v>
+        <v>271</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>114</v>
+        <v>270</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>115</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-    </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="A47" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>108</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="C96" s="2" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B98" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-    </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B103" s="4"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>